<commit_message>
add custom knowleadge selection and integrate it with the chatbot
</commit_message>
<xml_diff>
--- a/src/data/empty_data.xlsx
+++ b/src/data/empty_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/914d435ab6fbacf7/Área de Trabalho/New folder (2)/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F3905CD-17DC-4FD3-B0F8-AA796C0E0F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{1F3905CD-17DC-4FD3-B0F8-AA796C0E0F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7335EAA-717B-47B7-B801-59C40CDBA537}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{2E1453AD-0B1C-444B-BC6C-7225B7BC8AE5}"/>
   </bookViews>
@@ -33,6 +33,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,12 +393,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B0E59A2-B22B-4A8D-98E2-0902CAAEB5D8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>